<commit_message>
Improvements & Bug Fixes
如題
</commit_message>
<xml_diff>
--- a/編碼修改記錄.xlsx
+++ b/編碼修改記錄.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369">
   <si>
     <t>汉字</t>
   </si>
@@ -8570,6 +8570,30 @@
   </si>
   <si>
     <t>kcpm</t>
+  </si>
+  <si>
+    <t>mrhkp</t>
+  </si>
+  <si>
+    <t>llme</t>
+  </si>
+  <si>
+    <t>mfvik</t>
+  </si>
+  <si>
+    <t>mfhg</t>
+  </si>
+  <si>
+    <t>雇</t>
+  </si>
+  <si>
+    <t>msog</t>
+  </si>
+  <si>
+    <t>mfhgr</t>
+  </si>
+  <si>
+    <t>llomv</t>
   </si>
   <si>
     <t>是否重碼</t>
@@ -10144,30 +10168,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -10175,8 +10175,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10198,7 +10221,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10213,18 +10268,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10237,38 +10284,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10283,103 +10307,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10391,61 +10325,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10463,7 +10349,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10477,11 +10501,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10501,21 +10564,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -10523,24 +10571,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10560,17 +10590,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10582,10 +10606,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -10594,67 +10618,85 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -10663,40 +10705,10 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -10708,19 +10720,31 @@
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -11764,7 +11788,7 @@
   <dimension ref="A2:F1438"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1412" workbookViewId="0">
-      <selection activeCell="C1427" sqref="C1427"/>
+      <selection activeCell="B1431" sqref="B1431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -28244,39 +28268,81 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="1428" spans="2:2">
+    <row r="1428" spans="1:3">
+      <c r="A1428" t="s">
+        <v>584</v>
+      </c>
       <c r="B1428" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1429" spans="2:2">
+      <c r="C1428" t="s">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:3">
+      <c r="A1429" t="s">
+        <v>1195</v>
+      </c>
       <c r="B1429" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1430" spans="2:2">
+      <c r="C1429" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:3">
+      <c r="A1430" t="s">
+        <v>667</v>
+      </c>
       <c r="B1430" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1431" spans="2:2">
+      <c r="C1430" t="s">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:3">
+      <c r="A1431" t="s">
+        <v>663</v>
+      </c>
       <c r="B1431" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1432" spans="2:2">
+      <c r="C1431" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:3">
+      <c r="A1432" t="s">
+        <v>2854</v>
+      </c>
       <c r="B1432" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1433" spans="2:2">
+      <c r="C1432" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:3">
+      <c r="A1433" t="s">
+        <v>713</v>
+      </c>
       <c r="B1433" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="1434" spans="2:2">
+      <c r="C1433" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:3">
+      <c r="A1434" t="s">
+        <v>1201</v>
+      </c>
       <c r="B1434" t="s">
         <v>164</v>
+      </c>
+      <c r="C1434" t="s">
+        <v>2857</v>
       </c>
     </row>
     <row r="1435" spans="2:2">
@@ -28311,38 +28377,38 @@
   <sheetPr/>
   <dimension ref="A1:D305"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>2850</v>
+        <v>2858</v>
       </c>
       <c r="C1" t="s">
-        <v>2851</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2852</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2853</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2854</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>2855</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -28352,72 +28418,72 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>2856</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>2857</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>2858</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>2859</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>2860</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>2861</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>2862</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>2863</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>2864</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>2865</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>2866</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>2867</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>2868</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>2869</v>
+        <v>2877</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
@@ -28425,62 +28491,62 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>2870</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>2871</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>2872</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>2873</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>2874</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>2875</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>2876</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>2877</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>2878</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>2879</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>2880</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>2881</v>
+        <v>2889</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
@@ -28488,32 +28554,32 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>2882</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>2883</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>2884</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>2885</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>2886</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>2887</v>
+        <v>2895</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
@@ -28521,7 +28587,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>2888</v>
+        <v>2896</v>
       </c>
       <c r="B39" t="s">
         <v>60</v>
@@ -28529,77 +28595,77 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>2889</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>2890</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>2891</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>2892</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>2893</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>2894</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>2895</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>2896</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>2897</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>2898</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>2899</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>2900</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>2901</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>2902</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>2903</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="55" spans="1:1">
@@ -28609,57 +28675,57 @@
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>2904</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>2905</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>2906</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>2907</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>2908</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>2909</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>2910</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>2911</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>2912</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>2913</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>2914</v>
+        <v>2922</v>
       </c>
       <c r="B66" t="s">
         <v>60</v>
@@ -28667,27 +28733,27 @@
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>2915</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>2916</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>2917</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>2918</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>2919</v>
+        <v>2927</v>
       </c>
       <c r="B71" t="s">
         <v>64</v>
@@ -28695,32 +28761,32 @@
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>2920</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>2921</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>2922</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>2923</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>2924</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>2925</v>
+        <v>2933</v>
       </c>
       <c r="B77" t="s">
         <v>60</v>
@@ -28728,27 +28794,27 @@
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>2926</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>2927</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>2928</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>2929</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>2930</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="83" spans="1:1">
@@ -28771,7 +28837,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>2931</v>
+        <v>2939</v>
       </c>
       <c r="B86" t="s">
         <v>60</v>
@@ -28794,7 +28860,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>2932</v>
+        <v>2940</v>
       </c>
       <c r="B90" t="s">
         <v>60</v>
@@ -28802,7 +28868,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>2933</v>
+        <v>2941</v>
       </c>
       <c r="B91" t="s">
         <v>60</v>
@@ -28810,95 +28876,95 @@
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>2934</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>2935</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>2936</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>2937</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>2938</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>2939</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>2940</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>2941</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>2942</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>2943</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>2944</v>
+        <v>2952</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>2945</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>2946</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>2947</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>2948</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>2949</v>
+        <v>2957</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>2950</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>2951</v>
+        <v>2959</v>
       </c>
       <c r="B109" t="s">
-        <v>2952</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="110" spans="1:1">
@@ -28908,27 +28974,27 @@
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>2953</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>2954</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>2955</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>2956</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>2957</v>
+        <v>2965</v>
       </c>
       <c r="B115" t="s">
         <v>60</v>
@@ -28936,22 +29002,22 @@
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>2958</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>2959</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>2960</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>2961</v>
+        <v>2969</v>
       </c>
       <c r="B119" t="s">
         <v>64</v>
@@ -28959,7 +29025,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>2962</v>
+        <v>2970</v>
       </c>
       <c r="B120" t="s">
         <v>60</v>
@@ -28967,107 +29033,107 @@
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>2963</v>
+        <v>2971</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>2964</v>
+        <v>2972</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>2965</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>2966</v>
+        <v>2974</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>2967</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>2968</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>2969</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>2970</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>2971</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>2972</v>
+        <v>2980</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>2973</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>2974</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>2975</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>2976</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>2977</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>2978</v>
+        <v>2986</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>2979</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>2980</v>
+        <v>2988</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>2981</v>
+        <v>2989</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>2982</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>2983</v>
+        <v>2991</v>
       </c>
       <c r="B141" t="s">
         <v>60</v>
@@ -29075,12 +29141,12 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>2984</v>
+        <v>2992</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>2985</v>
+        <v>2993</v>
       </c>
       <c r="B143" t="s">
         <v>1845</v>
@@ -29088,7 +29154,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>2986</v>
+        <v>2994</v>
       </c>
       <c r="B144" t="s">
         <v>60</v>
@@ -29096,47 +29162,47 @@
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>2987</v>
+        <v>2995</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>2988</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>2989</v>
+        <v>2997</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>2990</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>2991</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>2992</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>2993</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>2994</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>2995</v>
+        <v>3003</v>
       </c>
       <c r="B153" t="s">
         <v>60</v>
@@ -29144,17 +29210,17 @@
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>2996</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>2997</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>2998</v>
+        <v>3006</v>
       </c>
       <c r="B156" t="s">
         <v>64</v>
@@ -29162,42 +29228,42 @@
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>2999</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>3000</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>3001</v>
+        <v>3009</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>3002</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>3003</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>3004</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>3005</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>3006</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="165" spans="1:1">
@@ -29207,7 +29273,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>3007</v>
+        <v>3015</v>
       </c>
       <c r="B166" t="s">
         <v>60</v>
@@ -29215,37 +29281,37 @@
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>3008</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>3009</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>3010</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>3011</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>3012</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>3013</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>3014</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="174" spans="1:1">
@@ -29255,17 +29321,17 @@
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>3015</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>3016</v>
+        <v>3024</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>3017</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="178" spans="1:1">
@@ -29275,12 +29341,12 @@
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>3018</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>3019</v>
+        <v>3027</v>
       </c>
       <c r="B180" t="s">
         <v>64</v>
@@ -29288,12 +29354,12 @@
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>3020</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>3021</v>
+        <v>3029</v>
       </c>
       <c r="B182" t="s">
         <v>60</v>
@@ -29301,30 +29367,30 @@
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>3022</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>3023</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>3024</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>3025</v>
+        <v>3033</v>
       </c>
       <c r="B186" t="s">
-        <v>3026</v>
+        <v>3034</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>3027</v>
+        <v>3035</v>
       </c>
       <c r="B187" t="s">
         <v>64</v>
@@ -29332,52 +29398,52 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>3028</v>
+        <v>3036</v>
       </c>
       <c r="B188" t="s">
-        <v>3029</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>3030</v>
+        <v>3038</v>
       </c>
       <c r="B189" t="s">
-        <v>3031</v>
+        <v>3039</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>3032</v>
+        <v>3040</v>
       </c>
       <c r="B190" t="s">
-        <v>3029</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>3033</v>
+        <v>3041</v>
       </c>
       <c r="B191" t="s">
-        <v>3034</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>3035</v>
+        <v>3043</v>
       </c>
       <c r="B192" t="s">
-        <v>3036</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>3037</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>3038</v>
+        <v>3046</v>
       </c>
       <c r="B194" t="s">
         <v>60</v>
@@ -29385,23 +29451,23 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>3039</v>
+        <v>3047</v>
       </c>
       <c r="B195" t="s">
-        <v>3034</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>3040</v>
+        <v>3048</v>
       </c>
       <c r="B196" t="s">
-        <v>3034</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>3041</v>
+        <v>3049</v>
       </c>
       <c r="B197" t="s">
         <v>60</v>
@@ -29409,25 +29475,25 @@
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>3042</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>3043</v>
+        <v>3051</v>
       </c>
       <c r="B199" t="s">
-        <v>3044</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>3045</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>3046</v>
+        <v>3054</v>
       </c>
       <c r="B201" t="s">
         <v>64</v>
@@ -29435,55 +29501,55 @@
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>3047</v>
+        <v>3055</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>3048</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>3049</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>3050</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>3051</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>3052</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>3053</v>
+        <v>3061</v>
       </c>
       <c r="B208" t="s">
-        <v>3054</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>3055</v>
+        <v>3063</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>3056</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>3057</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -29496,17 +29562,17 @@
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>3058</v>
+        <v>3066</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>3059</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>3060</v>
+        <v>3068</v>
       </c>
       <c r="B215" t="s">
         <v>64</v>
@@ -29514,27 +29580,27 @@
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>3061</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>3062</v>
+        <v>3070</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>3063</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>3064</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>3065</v>
+        <v>3073</v>
       </c>
       <c r="B220" t="s">
         <v>64</v>
@@ -29542,87 +29608,87 @@
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>3066</v>
+        <v>3074</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>3067</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>3068</v>
+        <v>3076</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>3069</v>
+        <v>3077</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>3070</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>3071</v>
+        <v>3079</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>3072</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>3073</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>3074</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>3075</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>3076</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>3077</v>
+        <v>3085</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>3078</v>
+        <v>3086</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>3079</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>3080</v>
+        <v>3088</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>3081</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>3082</v>
+        <v>3090</v>
       </c>
       <c r="B237" t="s">
         <v>407</v>
@@ -29630,21 +29696,21 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>3083</v>
+        <v>3091</v>
       </c>
       <c r="B238" t="s">
         <v>1228</v>
       </c>
       <c r="C238" t="s">
-        <v>3084</v>
+        <v>3092</v>
       </c>
       <c r="D238" t="s">
-        <v>3085</v>
+        <v>3093</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>3086</v>
+        <v>3094</v>
       </c>
       <c r="B239" t="s">
         <v>60</v>
@@ -29652,32 +29718,32 @@
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>3087</v>
+        <v>3095</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>3088</v>
+        <v>3096</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>3089</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>3090</v>
+        <v>3098</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>3091</v>
+        <v>3099</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>3092</v>
+        <v>3100</v>
       </c>
       <c r="B245" t="s">
         <v>64</v>
@@ -29685,7 +29751,7 @@
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>3093</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="247" spans="1:1">
@@ -29695,12 +29761,12 @@
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>3094</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>3095</v>
+        <v>3103</v>
       </c>
       <c r="B249" t="s">
         <v>64</v>
@@ -29708,7 +29774,7 @@
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>3096</v>
+        <v>3104</v>
       </c>
       <c r="B250" t="s">
         <v>60</v>
@@ -29716,17 +29782,17 @@
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>3097</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>3098</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>3099</v>
+        <v>3107</v>
       </c>
       <c r="B253" t="s">
         <v>60</v>
@@ -29734,7 +29800,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>3100</v>
+        <v>3108</v>
       </c>
       <c r="B254" t="s">
         <v>1845</v>
@@ -29742,22 +29808,22 @@
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>3101</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>3102</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>3103</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>3104</v>
+        <v>3112</v>
       </c>
       <c r="B258" t="s">
         <v>137</v>
@@ -29765,7 +29831,7 @@
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>3105</v>
+        <v>3113</v>
       </c>
       <c r="B259" t="s">
         <v>64</v>
@@ -29773,7 +29839,7 @@
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>3106</v>
+        <v>3114</v>
       </c>
       <c r="B260" t="s">
         <v>137</v>
@@ -29781,27 +29847,27 @@
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>3107</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>3108</v>
+        <v>3116</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>3109</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>3110</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>3111</v>
+        <v>3119</v>
       </c>
       <c r="B265" t="s">
         <v>64</v>
@@ -29809,7 +29875,7 @@
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>3112</v>
+        <v>3120</v>
       </c>
     </row>
     <row r="267" spans="1:1">
@@ -29819,17 +29885,17 @@
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>3113</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>3114</v>
+        <v>3122</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>3115</v>
+        <v>3123</v>
       </c>
       <c r="B270" t="s">
         <v>60</v>
@@ -29837,32 +29903,32 @@
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>3116</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>3117</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>3118</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>3119</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>3120</v>
+        <v>3128</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>3121</v>
+        <v>3129</v>
       </c>
       <c r="B276" t="s">
         <v>1845</v>
@@ -29870,33 +29936,33 @@
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>3122</v>
+        <v>3130</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>3123</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>3124</v>
+        <v>3132</v>
       </c>
       <c r="B279" t="s">
         <v>60</v>
       </c>
       <c r="C279" t="s">
-        <v>3125</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>3126</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>3127</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="282" spans="1:1">
@@ -29906,7 +29972,7 @@
     </row>
     <row r="283" spans="1:2">
       <c r="A283" t="s">
-        <v>3128</v>
+        <v>3136</v>
       </c>
       <c r="B283" t="s">
         <v>60</v>
@@ -29953,12 +30019,12 @@
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>3129</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" t="s">
-        <v>3130</v>
+        <v>3138</v>
       </c>
       <c r="B291" t="s">
         <v>60</v>
@@ -29966,27 +30032,27 @@
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>3131</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>3132</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>3133</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>3134</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" t="s">
-        <v>3135</v>
+        <v>3143</v>
       </c>
       <c r="B296" t="s">
         <v>64</v>
@@ -29994,35 +30060,35 @@
     </row>
     <row r="297" spans="1:2">
       <c r="A297" t="s">
-        <v>3136</v>
+        <v>3144</v>
       </c>
       <c r="B297" t="s">
-        <v>3137</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>3138</v>
+        <v>3146</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>3139</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>3140</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>3141</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" t="s">
-        <v>3142</v>
+        <v>3150</v>
       </c>
       <c r="B302" t="s">
         <v>137</v>
@@ -30030,7 +30096,7 @@
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>3143</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="304" spans="1:1">
@@ -30040,7 +30106,7 @@
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>3144</v>
+        <v>3152</v>
       </c>
     </row>
   </sheetData>
@@ -30062,381 +30128,381 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>3145</v>
+        <v>3153</v>
       </c>
       <c r="C1" t="s">
-        <v>3146</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3147</v>
+        <v>3155</v>
       </c>
       <c r="B2" t="s">
-        <v>3148</v>
+        <v>3156</v>
       </c>
       <c r="C2" t="s">
-        <v>3149</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" t="s">
-        <v>3150</v>
+        <v>3158</v>
       </c>
       <c r="C3" t="s">
-        <v>3151</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>3152</v>
+        <v>3160</v>
       </c>
       <c r="C4" t="s">
-        <v>3153</v>
+        <v>3161</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>3154</v>
+        <v>3162</v>
       </c>
       <c r="C5" t="s">
-        <v>3155</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" t="s">
-        <v>3156</v>
+        <v>3164</v>
       </c>
       <c r="C6" t="s">
-        <v>3157</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>3158</v>
+        <v>3166</v>
       </c>
       <c r="C7" t="s">
-        <v>3159</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>3160</v>
+        <v>3168</v>
       </c>
       <c r="C8" t="s">
-        <v>3161</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>3162</v>
+        <v>3170</v>
       </c>
       <c r="C9" t="s">
-        <v>3163</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>3164</v>
+        <v>3172</v>
       </c>
       <c r="C10" t="s">
-        <v>3165</v>
+        <v>3173</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>3166</v>
+        <v>3174</v>
       </c>
       <c r="C11" t="s">
-        <v>3167</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>3168</v>
+        <v>3176</v>
       </c>
       <c r="C12" t="s">
-        <v>3169</v>
+        <v>3177</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>3170</v>
+        <v>3178</v>
       </c>
       <c r="C13" t="s">
-        <v>3171</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>3172</v>
+        <v>3180</v>
       </c>
       <c r="C14" t="s">
-        <v>3173</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>3174</v>
+        <v>3182</v>
       </c>
       <c r="C15" t="s">
-        <v>3175</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>3176</v>
+        <v>3184</v>
       </c>
       <c r="C16" t="s">
-        <v>3175</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>3177</v>
+        <v>3185</v>
       </c>
       <c r="C17" t="s">
-        <v>3178</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>3179</v>
+        <v>3187</v>
       </c>
       <c r="C18" t="s">
-        <v>3180</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>3181</v>
+        <v>3189</v>
       </c>
       <c r="C19" t="s">
-        <v>3182</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>3183</v>
+        <v>3191</v>
       </c>
       <c r="C20" t="s">
-        <v>3184</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>3185</v>
+        <v>3193</v>
       </c>
       <c r="C21" t="s">
-        <v>3186</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>3187</v>
+        <v>3195</v>
       </c>
       <c r="C22" t="s">
-        <v>3188</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>3189</v>
+        <v>3197</v>
       </c>
       <c r="C23" t="s">
-        <v>3190</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>3191</v>
+        <v>3199</v>
       </c>
       <c r="C24" t="s">
-        <v>3192</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>3193</v>
+        <v>3201</v>
       </c>
       <c r="C25" t="s">
-        <v>3194</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>3195</v>
+        <v>3203</v>
       </c>
       <c r="C26" t="s">
-        <v>3196</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" t="s">
-        <v>3197</v>
+        <v>3205</v>
       </c>
       <c r="C27" t="s">
-        <v>3198</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" t="s">
-        <v>3199</v>
+        <v>3207</v>
       </c>
       <c r="C28" t="s">
-        <v>3200</v>
+        <v>3208</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" t="s">
-        <v>3201</v>
+        <v>3209</v>
       </c>
       <c r="C29" t="s">
-        <v>3202</v>
+        <v>3210</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>3203</v>
+        <v>3211</v>
       </c>
       <c r="C30" t="s">
-        <v>3204</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="B31" t="s">
-        <v>3205</v>
+        <v>3213</v>
       </c>
       <c r="C31" t="s">
-        <v>3206</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" t="s">
-        <v>3207</v>
+        <v>3215</v>
       </c>
       <c r="C32" t="s">
-        <v>3208</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>3209</v>
+        <v>3217</v>
       </c>
       <c r="C33" t="s">
-        <v>3210</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>3211</v>
+        <v>3219</v>
       </c>
       <c r="C34" t="s">
-        <v>3212</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>3213</v>
+        <v>3221</v>
       </c>
       <c r="C35" t="s">
-        <v>3214</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" t="s">
-        <v>3215</v>
+        <v>3223</v>
       </c>
       <c r="C36" t="s">
-        <v>3216</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>3217</v>
+        <v>3225</v>
       </c>
       <c r="C37" t="s">
-        <v>3218</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>3219</v>
+        <v>3227</v>
       </c>
       <c r="C38" t="s">
-        <v>3220</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>3221</v>
+        <v>3229</v>
       </c>
       <c r="C39" t="s">
-        <v>3222</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>3223</v>
+        <v>3231</v>
       </c>
       <c r="C40" t="s">
-        <v>3224</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>3225</v>
+        <v>3233</v>
       </c>
       <c r="C41" t="s">
-        <v>3226</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>3227</v>
+        <v>3235</v>
       </c>
       <c r="C42" t="s">
-        <v>3228</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>3229</v>
+        <v>3237</v>
       </c>
       <c r="C43" t="s">
-        <v>3230</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" t="s">
-        <v>3231</v>
+        <v>3239</v>
       </c>
       <c r="C44" t="s">
-        <v>3232</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>3233</v>
+        <v>3241</v>
       </c>
       <c r="C45" t="s">
-        <v>3234</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>3235</v>
+        <v>3243</v>
       </c>
       <c r="C46" t="s">
-        <v>3236</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>3237</v>
+        <v>3245</v>
       </c>
       <c r="C47" t="s">
-        <v>3238</v>
+        <v>3246</v>
       </c>
     </row>
   </sheetData>
@@ -30458,10 +30524,10 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>3239</v>
+        <v>3247</v>
       </c>
       <c r="C1" t="s">
-        <v>3240</v>
+        <v>3248</v>
       </c>
     </row>
   </sheetData>
@@ -30483,7 +30549,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3241</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -30520,112 +30586,112 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>3242</v>
+        <v>3250</v>
       </c>
       <c r="C1" t="s">
-        <v>3243</v>
+        <v>3251</v>
       </c>
       <c r="D1" t="s">
-        <v>3244</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3245</v>
+        <v>3253</v>
       </c>
       <c r="B2" t="s">
         <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>3246</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3247</v>
+        <v>3255</v>
       </c>
       <c r="B3" t="s">
         <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>3248</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3249</v>
+        <v>3257</v>
       </c>
       <c r="B4" t="s">
         <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>3250</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3251</v>
+        <v>3259</v>
       </c>
       <c r="B5" t="s">
         <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>3252</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>3253</v>
+        <v>3261</v>
       </c>
       <c r="B6" t="s">
         <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>3254</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3255</v>
+        <v>3263</v>
       </c>
       <c r="B7" t="s">
         <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>3256</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>3257</v>
+        <v>3265</v>
       </c>
       <c r="B8" t="s">
         <v>164</v>
       </c>
       <c r="C8" t="s">
-        <v>3258</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>3259</v>
+        <v>3267</v>
       </c>
       <c r="B9" t="s">
         <v>164</v>
       </c>
       <c r="C9" t="s">
-        <v>3260</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>3261</v>
+        <v>3269</v>
       </c>
       <c r="B10" t="s">
         <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>3262</v>
+        <v>3270</v>
       </c>
       <c r="D10" t="s">
         <v>60</v>
@@ -30633,101 +30699,101 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>3263</v>
+        <v>3271</v>
       </c>
       <c r="B11" t="s">
         <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>3264</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>3265</v>
+        <v>3273</v>
       </c>
       <c r="B12" t="s">
         <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>3266</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>3267</v>
+        <v>3275</v>
       </c>
       <c r="B13" t="s">
         <v>164</v>
       </c>
       <c r="C13" t="s">
-        <v>3268</v>
+        <v>3276</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3269</v>
+        <v>3277</v>
       </c>
       <c r="B14" t="s">
         <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>3270</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>3271</v>
+        <v>3279</v>
       </c>
       <c r="B15" t="s">
         <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>3272</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>3273</v>
+        <v>3281</v>
       </c>
       <c r="B16" t="s">
         <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>3274</v>
+        <v>3282</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>3275</v>
+        <v>3283</v>
       </c>
       <c r="B17" t="s">
         <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>3276</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>3277</v>
+        <v>3285</v>
       </c>
       <c r="B18" t="s">
         <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>3278</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>3279</v>
+        <v>3287</v>
       </c>
       <c r="B19" t="s">
         <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>3280</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -30738,7 +30804,7 @@
         <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>3281</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -30749,62 +30815,62 @@
         <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>3282</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>3283</v>
+        <v>3291</v>
       </c>
       <c r="B22" t="s">
         <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>3284</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>3285</v>
+        <v>3293</v>
       </c>
       <c r="B23" t="s">
         <v>164</v>
       </c>
       <c r="C23" t="s">
-        <v>3286</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>3287</v>
+        <v>3295</v>
       </c>
       <c r="B24" t="s">
         <v>164</v>
       </c>
       <c r="C24" t="s">
-        <v>3288</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>3289</v>
+        <v>3297</v>
       </c>
       <c r="B25" t="s">
         <v>164</v>
       </c>
       <c r="C25" t="s">
-        <v>3290</v>
+        <v>3298</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>3291</v>
+        <v>3299</v>
       </c>
       <c r="B26" t="s">
         <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>3292</v>
+        <v>3300</v>
       </c>
       <c r="D26" t="s">
         <v>60</v>
@@ -30812,35 +30878,35 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>3293</v>
+        <v>3301</v>
       </c>
       <c r="B27" t="s">
         <v>164</v>
       </c>
       <c r="C27" t="s">
-        <v>3294</v>
+        <v>3302</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>3295</v>
+        <v>3303</v>
       </c>
       <c r="B28" t="s">
         <v>164</v>
       </c>
       <c r="C28" t="s">
-        <v>3296</v>
+        <v>3304</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>3297</v>
+        <v>3305</v>
       </c>
       <c r="B29" t="s">
         <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>3298</v>
+        <v>3306</v>
       </c>
       <c r="D29" t="s">
         <v>60</v>
@@ -30848,68 +30914,68 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>3299</v>
+        <v>3307</v>
       </c>
       <c r="B30" t="s">
         <v>164</v>
       </c>
       <c r="C30" t="s">
-        <v>3300</v>
+        <v>3308</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>3301</v>
+        <v>3309</v>
       </c>
       <c r="B31" t="s">
         <v>164</v>
       </c>
       <c r="C31" t="s">
-        <v>3302</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>3303</v>
+        <v>3311</v>
       </c>
       <c r="B32" t="s">
         <v>164</v>
       </c>
       <c r="C32" t="s">
-        <v>3304</v>
+        <v>3312</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>3305</v>
+        <v>3313</v>
       </c>
       <c r="B33" t="s">
         <v>164</v>
       </c>
       <c r="C33" t="s">
-        <v>3306</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>3307</v>
+        <v>3315</v>
       </c>
       <c r="B34" t="s">
         <v>164</v>
       </c>
       <c r="C34" t="s">
-        <v>3308</v>
+        <v>3316</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>3309</v>
+        <v>3317</v>
       </c>
       <c r="B35" t="s">
         <v>164</v>
       </c>
       <c r="C35" t="s">
-        <v>3310</v>
+        <v>3318</v>
       </c>
       <c r="D35" t="s">
         <v>60</v>
@@ -30917,57 +30983,57 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>3311</v>
+        <v>3319</v>
       </c>
       <c r="B36" t="s">
         <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>3312</v>
+        <v>3320</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>3313</v>
+        <v>3321</v>
       </c>
       <c r="B37" t="s">
         <v>164</v>
       </c>
       <c r="C37" t="s">
-        <v>3314</v>
+        <v>3322</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>3315</v>
+        <v>3323</v>
       </c>
       <c r="B38" t="s">
         <v>164</v>
       </c>
       <c r="C38" t="s">
-        <v>3316</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>3317</v>
+        <v>3325</v>
       </c>
       <c r="B39" t="s">
         <v>164</v>
       </c>
       <c r="C39" t="s">
-        <v>3318</v>
+        <v>3326</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>3319</v>
+        <v>3327</v>
       </c>
       <c r="B40" t="s">
         <v>164</v>
       </c>
       <c r="C40" t="s">
-        <v>3320</v>
+        <v>3328</v>
       </c>
       <c r="D40" t="s">
         <v>60</v>
@@ -30975,13 +31041,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>3321</v>
+        <v>3329</v>
       </c>
       <c r="B41" t="s">
         <v>164</v>
       </c>
       <c r="C41" t="s">
-        <v>3320</v>
+        <v>3328</v>
       </c>
       <c r="D41" t="s">
         <v>407</v>
@@ -30989,68 +31055,68 @@
     </row>
     <row r="42" ht="18.75" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>3322</v>
+        <v>3330</v>
       </c>
       <c r="B42" t="s">
         <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>3323</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>3324</v>
+        <v>3332</v>
       </c>
       <c r="B43" t="s">
         <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>3325</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>3326</v>
+        <v>3334</v>
       </c>
       <c r="B44" t="s">
         <v>164</v>
       </c>
       <c r="C44" t="s">
-        <v>3327</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>3328</v>
+        <v>3336</v>
       </c>
       <c r="B45" t="s">
         <v>164</v>
       </c>
       <c r="C45" t="s">
-        <v>3329</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>3330</v>
+        <v>3338</v>
       </c>
       <c r="B46" t="s">
         <v>164</v>
       </c>
       <c r="C46" t="s">
-        <v>3331</v>
+        <v>3339</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>3332</v>
+        <v>3340</v>
       </c>
       <c r="B47" t="s">
         <v>164</v>
       </c>
       <c r="C47" t="s">
-        <v>3331</v>
+        <v>3339</v>
       </c>
       <c r="D47" t="s">
         <v>60</v>
@@ -31058,123 +31124,123 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>3333</v>
+        <v>3341</v>
       </c>
       <c r="B48" t="s">
         <v>164</v>
       </c>
       <c r="C48" t="s">
-        <v>3334</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>3335</v>
+        <v>3343</v>
       </c>
       <c r="B49" t="s">
         <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>3336</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>3337</v>
+        <v>3345</v>
       </c>
       <c r="B50" t="s">
         <v>164</v>
       </c>
       <c r="C50" t="s">
-        <v>3338</v>
+        <v>3346</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>3339</v>
+        <v>3347</v>
       </c>
       <c r="B51" t="s">
         <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>3340</v>
+        <v>3348</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>3341</v>
+        <v>3349</v>
       </c>
       <c r="B52" t="s">
         <v>164</v>
       </c>
       <c r="C52" t="s">
-        <v>3342</v>
+        <v>3350</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>3343</v>
+        <v>3351</v>
       </c>
       <c r="B53" t="s">
         <v>164</v>
       </c>
       <c r="C53" t="s">
-        <v>3344</v>
+        <v>3352</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>3345</v>
+        <v>3353</v>
       </c>
       <c r="B54" t="s">
         <v>164</v>
       </c>
       <c r="C54" t="s">
-        <v>3346</v>
+        <v>3354</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>3347</v>
+        <v>3355</v>
       </c>
       <c r="B55" t="s">
         <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>3348</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>3349</v>
+        <v>3357</v>
       </c>
       <c r="B56" t="s">
         <v>164</v>
       </c>
       <c r="C56" t="s">
-        <v>3350</v>
+        <v>3358</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>3351</v>
+        <v>3359</v>
       </c>
       <c r="B57" t="s">
         <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>3352</v>
+        <v>3360</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>3353</v>
+        <v>3361</v>
       </c>
       <c r="B58" t="s">
         <v>164</v>
       </c>
       <c r="C58" t="s">
-        <v>3354</v>
+        <v>3362</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -31182,13 +31248,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>3355</v>
+        <v>3363</v>
       </c>
       <c r="B59" t="s">
         <v>164</v>
       </c>
       <c r="C59" t="s">
-        <v>3356</v>
+        <v>3364</v>
       </c>
       <c r="D59" t="s">
         <v>60</v>
@@ -31196,7 +31262,7 @@
     </row>
     <row r="60" ht="18.75" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>3357</v>
+        <v>3365</v>
       </c>
       <c r="B60" t="s">
         <v>164</v>
@@ -31210,18 +31276,18 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>3358</v>
+        <v>3366</v>
       </c>
       <c r="B61" t="s">
         <v>164</v>
       </c>
       <c r="C61" t="s">
-        <v>3359</v>
+        <v>3367</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>3360</v>
+        <v>3368</v>
       </c>
       <c r="B62" t="s">
         <v>164</v>

</xml_diff>